<commit_message>
POc done, starting documentation to expose it
</commit_message>
<xml_diff>
--- a/results/ML/MLR_cEnroll_nPSU_nS1S2_vs_Desertor/backwardElimination.xlsx
+++ b/results/ML/MLR_cEnroll_nPSU_nS1S2_vs_Desertor/backwardElimination.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\models\desertorstudent\results\ML\MLR_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF76C83B-24FD-4478-9681-61F70B4C5826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EBFDD2-9F22-4EC5-80E3-0CABC0418C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="0" windowWidth="12000" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
 Model:                            OLS   Adj. R-squared:                  0.455
 Method:                 Least Squares   F-statistic:                     10.72
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):           2.01e-49
-Time:                        20:51:34   Log-Likelihood:                -153.95
+Time:                        20:59:35   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             401.9
 Df Residuals:                     490   BIC:                             603.3
 Df Model:                          46                                         
@@ -273,7 +273,7 @@
 Model:                            OLS   Adj. R-squared:                  0.456
 Method:                 Least Squares   F-statistic:                     10.98
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):           6.03e-50
-Time:                        20:51:34   Log-Likelihood:                -153.95
+Time:                        20:59:36   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             399.9
 Df Residuals:                     491   BIC:                             597.1
 Df Model:                          45                                         
@@ -345,7 +345,7 @@
 Model:                            OLS   Adj. R-squared:                  0.457
 Method:                 Least Squares   F-statistic:                     11.25
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):           1.78e-50
-Time:                        20:51:34   Log-Likelihood:                -153.95
+Time:                        20:59:36   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             397.9
 Df Residuals:                     492   BIC:                             590.8
 Df Model:                          44                                         
@@ -416,7 +416,7 @@
 Model:                            OLS   Adj. R-squared:                  0.458
 Method:                 Least Squares   F-statistic:                     11.54
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):           5.22e-51
-Time:                        20:51:34   Log-Likelihood:                -153.95
+Time:                        20:59:36   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             395.9
 Df Residuals:                     493   BIC:                             584.5
 Df Model:                          43                                         
@@ -486,7 +486,7 @@
 Model:                            OLS   Adj. R-squared:                  0.459
 Method:                 Least Squares   F-statistic:                     11.84
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):           1.51e-51
-Time:                        20:51:34   Log-Likelihood:                -153.95
+Time:                        20:59:36   Log-Likelihood:                -153.95
 No. Observations:                 537   AIC:                             393.9
 Df Residuals:                     494   BIC:                             578.2
 Df Model:                          42                                         
@@ -555,7 +555,7 @@
 Model:                            OLS   Adj. R-squared:                  0.460
 Method:                 Least Squares   F-statistic:                     12.15
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):           4.31e-52
-Time:                        20:51:34   Log-Likelihood:                -153.96
+Time:                        20:59:36   Log-Likelihood:                -153.96
 No. Observations:                 537   AIC:                             391.9
 Df Residuals:                     495   BIC:                             571.9
 Df Model:                          41                                         
@@ -623,7 +623,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.620
 Method:                 Least Squares   F-statistic:                              22.38
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    7.29e-88
-Time:                        20:51:34   Log-Likelihood:                         -153.99
+Time:                        20:59:36   Log-Likelihood:                         -153.99
 No. Observations:                 537   AIC:                                      390.0
 Df Residuals:                     496   BIC:                                      565.7
 Df Model:                          41                                                  
@@ -690,7 +690,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.621
 Method:                 Least Squares   F-statistic:                              22.98
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.53e-88
-Time:                        20:51:34   Log-Likelihood:                         -154.01
+Time:                        20:59:36   Log-Likelihood:                         -154.01
 No. Observations:                 537   AIC:                                      388.0
 Df Residuals:                     497   BIC:                                      559.5
 Df Model:                          40                                                  
@@ -756,7 +756,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.622
 Method:                 Least Squares   F-statistic:                              23.61
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    3.22e-89
-Time:                        20:51:34   Log-Likelihood:                         -154.04
+Time:                        20:59:36   Log-Likelihood:                         -154.04
 No. Observations:                 537   AIC:                                      386.1
 Df Residuals:                     498   BIC:                                      553.2
 Df Model:                          39                                                  
@@ -821,7 +821,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.622
 Method:                 Least Squares   F-statistic:                              24.28
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    6.53e-90
-Time:                        20:51:34   Log-Likelihood:                         -154.05
+Time:                        20:59:36   Log-Likelihood:                         -154.05
 No. Observations:                 537   AIC:                                      384.1
 Df Residuals:                     499   BIC:                                      547.0
 Df Model:                          38                                                  
@@ -885,7 +885,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.623
 Method:                 Least Squares   F-statistic:                              24.99
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.33e-90
-Time:                        20:51:34   Log-Likelihood:                         -154.08
+Time:                        20:59:36   Log-Likelihood:                         -154.08
 No. Observations:                 537   AIC:                                      382.2
 Df Residuals:                     500   BIC:                                      540.7
 Df Model:                          37                                                  
@@ -948,7 +948,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.624
 Method:                 Least Squares   F-statistic:                              25.73
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    2.69e-91
-Time:                        20:51:34   Log-Likelihood:                         -154.12
+Time:                        20:59:36   Log-Likelihood:                         -154.12
 No. Observations:                 537   AIC:                                      380.2
 Df Residuals:                     501   BIC:                                      534.5
 Df Model:                          36                                                  
@@ -1010,7 +1010,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.624
 Method:                 Least Squares   F-statistic:                              26.51
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    5.36e-92
-Time:                        20:51:34   Log-Likelihood:                         -154.15
+Time:                        20:59:36   Log-Likelihood:                         -154.15
 No. Observations:                 537   AIC:                                      378.3
 Df Residuals:                     502   BIC:                                      528.3
 Df Model:                          35                                                  
@@ -1071,7 +1071,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.625
 Method:                 Least Squares   F-statistic:                              27.33
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.07e-92
-Time:                        20:51:34   Log-Likelihood:                         -154.21
+Time:                        20:59:36   Log-Likelihood:                         -154.21
 No. Observations:                 537   AIC:                                      376.4
 Df Residuals:                     503   BIC:                                      522.1
 Df Model:                          34                                                  
@@ -1131,7 +1131,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.626
 Method:                 Least Squares   F-statistic:                              28.21
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    2.11e-93
-Time:                        20:51:34   Log-Likelihood:                         -154.27
+Time:                        20:59:36   Log-Likelihood:                         -154.27
 No. Observations:                 537   AIC:                                      374.5
 Df Residuals:                     504   BIC:                                      516.0
 Df Model:                          33                                                  
@@ -1190,7 +1190,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.626
 Method:                 Least Squares   F-statistic:                              29.13
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    4.23e-94
-Time:                        20:51:34   Log-Likelihood:                         -154.37
+Time:                        20:59:36   Log-Likelihood:                         -154.37
 No. Observations:                 537   AIC:                                      372.7
 Df Residuals:                     505   BIC:                                      509.9
 Df Model:                          32                                                  
@@ -1248,7 +1248,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.627
 Method:                 Least Squares   F-statistic:                              30.11
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    8.41e-95
-Time:                        20:51:34   Log-Likelihood:                         -154.48
+Time:                        20:59:36   Log-Likelihood:                         -154.48
 No. Observations:                 537   AIC:                                      371.0
 Df Residuals:                     506   BIC:                                      503.8
 Df Model:                          31                                                  
@@ -1305,7 +1305,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.627
 Method:                 Least Squares   F-statistic:                              31.15
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.67e-95
-Time:                        20:51:34   Log-Likelihood:                         -154.60
+Time:                        20:59:36   Log-Likelihood:                         -154.60
 No. Observations:                 537   AIC:                                      369.2
 Df Residuals:                     507   BIC:                                      497.8
 Df Model:                          30                                                  
@@ -1361,7 +1361,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.628
 Method:                 Least Squares   F-statistic:                              32.27
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    3.27e-96
-Time:                        20:51:34   Log-Likelihood:                         -154.73
+Time:                        20:59:36   Log-Likelihood:                         -154.73
 No. Observations:                 537   AIC:                                      367.5
 Df Residuals:                     508   BIC:                                      491.7
 Df Model:                          29                                                  
@@ -1416,7 +1416,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.628
 Method:                 Least Squares   F-statistic:                              33.44
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    7.05e-97
-Time:                        20:51:34   Log-Likelihood:                         -154.98
+Time:                        20:59:36   Log-Likelihood:                         -154.98
 No. Observations:                 537   AIC:                                      366.0
 Df Residuals:                     509   BIC:                                      486.0
 Df Model:                          28                                                  
@@ -1470,7 +1470,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.629
 Method:                 Least Squares   F-statistic:                              34.69
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.53e-97
-Time:                        20:51:34   Log-Likelihood:                         -155.25
+Time:                        20:59:36   Log-Likelihood:                         -155.25
 No. Observations:                 537   AIC:                                      364.5
 Df Residuals:                     510   BIC:                                      480.2
 Df Model:                          27                                                  
@@ -1523,7 +1523,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.629
 Method:                 Least Squares   F-statistic:                              36.05
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    3.04e-98
-Time:                        20:51:34   Log-Likelihood:                         -155.46
+Time:                        20:59:36   Log-Likelihood:                         -155.46
 No. Observations:                 537   AIC:                                      362.9
 Df Residuals:                     511   BIC:                                      474.4
 Df Model:                          26                                                  
@@ -1575,7 +1575,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              37.56
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    5.05e-99
-Time:                        20:51:35   Log-Likelihood:                         -155.49
+Time:                        20:59:36   Log-Likelihood:                         -155.49
 No. Observations:                 537   AIC:                                      361.0
 Df Residuals:                     512   BIC:                                      468.1
 Df Model:                          25                                                  
@@ -1626,7 +1626,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              39.12
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                    1.13e-99
-Time:                        20:51:35   Log-Likelihood:                         -155.87
+Time:                        20:59:36   Log-Likelihood:                         -155.87
 No. Observations:                 537   AIC:                                      359.7
 Df Residuals:                     513   BIC:                                      462.6
 Df Model:                          24                                                  
@@ -1676,7 +1676,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              40.79
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   2.71e-100
-Time:                        20:51:35   Log-Likelihood:                         -156.33
+Time:                        20:59:36   Log-Likelihood:                         -156.33
 No. Observations:                 537   AIC:                                      358.7
 Df Residuals:                     514   BIC:                                      457.2
 Df Model:                          23                                                  
@@ -1725,7 +1725,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              42.56
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   7.59e-101
-Time:                        20:51:35   Log-Likelihood:                         -156.99
+Time:                        20:59:36   Log-Likelihood:                         -156.99
 No. Observations:                 537   AIC:                                      358.0
 Df Residuals:                     515   BIC:                                      452.3
 Df Model:                          22                                                  
@@ -1773,7 +1773,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.630
 Method:                 Least Squares   F-statistic:                              44.50
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   2.16e-101
-Time:                        20:51:35   Log-Likelihood:                         -157.69
+Time:                        20:59:36   Log-Likelihood:                         -157.69
 No. Observations:                 537   AIC:                                      357.4
 Df Residuals:                     516   BIC:                                      447.4
 Df Model:                          21                                                  
@@ -1820,7 +1820,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.629
 Method:                 Least Squares   F-statistic:                              46.61
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   6.25e-102
-Time:                        20:51:35   Log-Likelihood:                         -158.43
+Time:                        20:59:36   Log-Likelihood:                         -158.43
 No. Observations:                 537   AIC:                                      356.9
 Df Residuals:                     517   BIC:                                      442.6
 Df Model:                          20                                                  
@@ -1866,7 +1866,7 @@
 Model:                            OLS   Adj. R-squared (uncentered):              0.627
 Method:                 Least Squares   F-statistic:                              51.23
 Date:                Sat, 28 Dec 2019   Prob (F-statistic):                   1.33e-102
-Time:                        20:51:35   Log-Likelihood:                         -160.96
+Time:                        20:59:36   Log-Likelihood:                         -160.96
 No. Observations:                 537   AIC:                                      357.9
 Df Residuals:                     519   BIC:                                      435.1
 Df Model:                          18                                                  

</xml_diff>